<commit_message>
testStats on Reports finished
</commit_message>
<xml_diff>
--- a/ProdFloor/wwwroot/Testingdummy.xlsx
+++ b/ProdFloor/wwwroot/Testingdummy.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
   <si>
     <t xml:space="preserve">PO</t>
   </si>
@@ -27,6 +27,18 @@
   </si>
   <si>
     <t xml:space="preserve">Tester Tech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELEM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELEM2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S11</t>
   </si>
   <si>
     <t xml:space="preserve">S4</t>
@@ -92,7 +104,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>3698741</v>
+        <v>3111112</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -103,12 +115,122 @@
     </row>
     <row r="3">
       <c r="A3">
+        <v>3002121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3000505</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>3215648</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>3698741</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>3222224</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>3222226</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>3333339</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>3333332</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>3333331</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>3333333</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
         <v>3439739</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>